<commit_message>
added parameter tuning & stratified k fold cross validation
</commit_message>
<xml_diff>
--- a/data/pseudo_data.xlsx
+++ b/data/pseudo_data.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgia/Documents/Capstone/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B6BBC1-CF83-9C42-BF31-D181CE35D3B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E672CAD0-C9DC-E546-BED6-427D7D329663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C717D2F8-7EC4-D944-B19C-5125B320A82B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{C717D2F8-7EC4-D944-B19C-5125B320A82B}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="210">
   <si>
     <t>Test Lead</t>
   </si>
@@ -654,13 +655,25 @@
   </si>
   <si>
     <t xml:space="preserve">Yes </t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Classification #3</t>
+  </si>
+  <si>
+    <t>Why defect was not identified during testing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -707,6 +720,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -749,7 +770,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -793,6 +814,13 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1109,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C58AB81-234C-4747-9504-4C13DE14D167}">
   <dimension ref="A1:G246"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="C209" sqref="C209"/>
+    <sheetView zoomScale="135" workbookViewId="0">
+      <selection activeCell="C232" sqref="C232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1736,7 +1764,7 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>197</v>
       </c>
@@ -1787,7 +1815,7 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" s="5" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" s="5" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>198</v>
       </c>
@@ -4855,6 +4883,129 @@
       </c>
       <c r="E246" s="2" t="s">
         <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93E853-69BD-B041-96BD-8740EF4EE202}">
+  <dimension ref="B2:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="3" max="3" width="52.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B5" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="16" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B10" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B11" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="B12" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="16" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented text augmentation & rerun models
</commit_message>
<xml_diff>
--- a/data/pseudo_data.xlsx
+++ b/data/pseudo_data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/georgia/Documents/Capstone/code/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E672CAD0-C9DC-E546-BED6-427D7D329663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBE8DBE-E00E-034A-8930-C1769E00B9BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{C717D2F8-7EC4-D944-B19C-5125B320A82B}"/>
   </bookViews>
   <sheets>
     <sheet name="Defect Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Base Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="208">
   <si>
     <t>Test Lead</t>
   </si>
@@ -655,12 +655,6 @@
   </si>
   <si>
     <t xml:space="preserve">Yes </t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Classification #3</t>
@@ -770,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -814,13 +808,19 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4892,121 +4892,118 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C93E853-69BD-B041-96BD-8740EF4EE202}">
-  <dimension ref="B2:C14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B2" s="15" t="s">
-        <v>208</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="16" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B4" s="16" t="s">
+    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="B3" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B5" s="16" t="s">
+    <row r="4" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="B4" s="18" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="16" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="B5" s="18" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="16" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="B6" s="18" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="16" t="s">
+    <row r="7" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="16" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="B8" s="18" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="16" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="B9" s="18" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B11" s="16" t="s">
+    <row r="10" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="B10" s="18" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="B12" s="16" t="s">
+    <row r="11" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C12" s="17" t="s">
+      <c r="B11" s="18" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B13" s="16" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="B12" s="18" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B14" s="16" t="s">
-        <v>206</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>207</v>
-      </c>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>